<commit_message>
next version. working toward working beta
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seedo\Documents\Coding\Random Projects\SMS Receiver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312A1173-E43D-45BD-9DEC-BC558103B82A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F16F226-D0D4-486E-BF85-A21E1C96A15A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{93B31EA7-6507-49EC-864E-A309B3F4DA42}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{93B31EA7-6507-49EC-864E-A309B3F4DA42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>app.py</t>
   </si>
@@ -100,9 +100,6 @@
     <t>game_of_things_questions.txt</t>
   </si>
   <si>
-    <t>answers.txt</t>
-  </si>
-  <si>
     <t>players.csv</t>
   </si>
   <si>
@@ -127,8 +124,104 @@
     <t>display_available_players()</t>
   </si>
   <si>
+    <t>add_player_answer(message_body)</t>
+  </si>
+  <si>
+    <t>Adds player answer to answers.txt</t>
+  </si>
+  <si>
+    <t>find_num_of_lines(file)</t>
+  </si>
+  <si>
+    <t>Opens given file and checks it's length.</t>
+  </si>
+  <si>
+    <t>get_random_question(file)</t>
+  </si>
+  <si>
+    <t>Retrieves a random question, checks if it has been used, returns string.</t>
+  </si>
+  <si>
+    <t>players (list), used_questions (list), question_file (string, 'game_of_things_questions.txt')</t>
+  </si>
+  <si>
+    <t>2. define starting variables</t>
+  </si>
+  <si>
+    <t>1. clear any used files</t>
+  </si>
+  <si>
+    <t>temp.txt, answers.txt, players.csv</t>
+  </si>
+  <si>
+    <t>3. sets 'name' as environmental variable</t>
+  </si>
+  <si>
+    <t>4. Print names to terminal as they file in.</t>
+  </si>
+  <si>
+    <t>SETUP</t>
+  </si>
+  <si>
+    <t>GAME</t>
+  </si>
+  <si>
+    <t>5. Change environmental variable to 'game'</t>
+  </si>
+  <si>
+    <t>TO DO</t>
+  </si>
+  <si>
+    <t>Replace env variable with simpler logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design </t>
+  </si>
+  <si>
+    <t>misc</t>
+  </si>
+  <si>
+    <t>6. Retrieve random question and print on screen while players input</t>
+  </si>
+  <si>
+    <t>Check input every 7 seconds to see if it all answers are in</t>
+  </si>
+  <si>
+    <t>display_question(current_question)</t>
+  </si>
+  <si>
+    <t>8. call out player if it takes more than 60 seconds for them to answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. allow force start </t>
+  </si>
+  <si>
+    <t>11. allow input for number answer</t>
+  </si>
+  <si>
+    <t>10. display all answers on screen (slow print each answer and use colors/bold to focus on each one.</t>
+  </si>
+  <si>
+    <t>12. start over from part 6</t>
+  </si>
+  <si>
+    <t>display.py</t>
+  </si>
+  <si>
+    <t>Design elements for the game that we pass info through</t>
+  </si>
+  <si>
+    <t>7. once input has reached players # animation that all questions are in</t>
+  </si>
+  <si>
+    <t>answers.py</t>
+  </si>
+  <si>
+    <t>next things start on players.py line 45</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Uses timer to print out the players as they are added to players.csv </t>
+      <t xml:space="preserve">prints out the players as they are added to players.csv </t>
     </r>
     <r>
       <rPr>
@@ -143,103 +236,19 @@
     </r>
   </si>
   <si>
-    <t>add_player_answer(message_body)</t>
-  </si>
-  <si>
-    <t>Adds player answer to answers.txt</t>
-  </si>
-  <si>
-    <t>….....input &gt;&gt; enter breaks refresh</t>
-  </si>
-  <si>
-    <t>find_num_of_lines(file)</t>
-  </si>
-  <si>
-    <t>Opens given file and checks it's length.</t>
-  </si>
-  <si>
-    <t>get_random_question(file)</t>
-  </si>
-  <si>
-    <t>Retrieves a random question, checks if it has been used, returns string.</t>
-  </si>
-  <si>
-    <t>players (list), used_questions (list), question_file (string, 'game_of_things_questions.txt')</t>
-  </si>
-  <si>
-    <t>2. define starting variables</t>
-  </si>
-  <si>
-    <t>1. clear any used files</t>
-  </si>
-  <si>
-    <t>temp.txt, answers.txt, players.csv</t>
-  </si>
-  <si>
-    <t>3. sets 'name' as environmental variable</t>
-  </si>
-  <si>
-    <t>4. Print names to terminal as they file in.</t>
-  </si>
-  <si>
-    <t>SETUP</t>
-  </si>
-  <si>
-    <t>GAME</t>
-  </si>
-  <si>
-    <t>5. Change environmental variable to 'game'</t>
-  </si>
-  <si>
-    <t>TO DO</t>
-  </si>
-  <si>
-    <t>Replace env variable with simpler logic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Design </t>
-  </si>
-  <si>
-    <t>misc</t>
-  </si>
-  <si>
-    <t>6. Retrieve random question and print on screen while players input</t>
-  </si>
-  <si>
-    <t>Check input every 7 seconds to see if it all answers are in</t>
-  </si>
-  <si>
-    <t>display_question(current_question)</t>
-  </si>
-  <si>
-    <t>8. call out player if it takes more than 60 seconds for them to answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9. allow force start </t>
-  </si>
-  <si>
-    <t>11. allow input for number answer</t>
-  </si>
-  <si>
-    <t>10. display all answers on screen (slow print each answer and use colors/bold to focus on each one.</t>
-  </si>
-  <si>
-    <t>12. start over from part 6</t>
-  </si>
-  <si>
-    <t>display.py</t>
-  </si>
-  <si>
-    <t>Design elements for the game that we pass info through</t>
-  </si>
-  <si>
-    <t>7. once input has reached players # animation that all questions are in</t>
-  </si>
-  <si>
-    <t>answers.py</t>
-  </si>
-  <si>
-    <t>next things start on players.py line 45</t>
+    <t>check_number_player()</t>
+  </si>
+  <si>
+    <t>check_number_answer()</t>
+  </si>
+  <si>
+    <t>checks to see if number has already been used for player</t>
+  </si>
+  <si>
+    <t>checks to see if number has already been used for answer</t>
+  </si>
+  <si>
+    <t>answers.csv</t>
   </si>
 </sst>
 </file>
@@ -665,20 +674,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A02626E-72DF-4602-B5F9-544756A8ECE8}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.1015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -689,10 +698,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -703,10 +712,10 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -714,10 +723,10 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -725,98 +734,101 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
         <v>55</v>
       </c>
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -824,104 +836,112 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="20" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B20" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
+    <row r="24" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B24" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="5" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>59</v>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more progress made. very close to an alpha build
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seedo\Documents\Coding\Random Projects\SMS Receiver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F16F226-D0D4-486E-BF85-A21E1C96A15A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7045B88-2143-408F-86C0-545037607738}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{93B31EA7-6507-49EC-864E-A309B3F4DA42}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{93B31EA7-6507-49EC-864E-A309B3F4DA42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A02626E-72DF-4602-B5F9-544756A8ECE8}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -909,33 +909,33 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" t="s">
-        <v>54</v>
-      </c>
-    </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>